<commit_message>
add create list and add item to list
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\github\buylist\BuyList\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t xml:space="preserve">Task </t>
   </si>
@@ -75,17 +75,23 @@
   </si>
   <si>
     <t>Allow merging (Appending lists)</t>
+  </si>
+  <si>
+    <t>show head line of list</t>
+  </si>
+  <si>
+    <t>view to show a list of lists in preview mode for select a list for edit.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -430,20 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="108.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="108.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -454,7 +460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -465,7 +471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -474,7 +480,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -485,7 +491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -494,7 +500,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -503,7 +509,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -512,7 +518,7 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -521,7 +527,7 @@
       </c>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -530,7 +536,7 @@
       </c>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -538,6 +544,16 @@
         <v>12</v>
       </c>
       <c r="C10" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>